<commit_message>
Updates to metadata and processing
Includes adjusting logger times to make sure all good 30 minute windows
are included in data analysis
</commit_message>
<xml_diff>
--- a/Metadata/LoggerTimes_Oceano.xlsx
+++ b/Metadata/LoggerTimes_Oceano.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="39140" yWindow="1140" windowWidth="25600" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1493,8 +1493,8 @@
   <dimension ref="A1:F172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G115" sqref="G115"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2482,7 +2482,7 @@
         <v>0.50277777777777777</v>
       </c>
       <c r="E49" s="8">
-        <v>0.77013888888888893</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="F49" s="2">
         <v>0</v>
@@ -3222,7 +3222,7 @@
         <v>0.56736111111111109</v>
       </c>
       <c r="E86" s="8">
-        <v>0.75555555555555554</v>
+        <v>0.75624999999999998</v>
       </c>
       <c r="F86" s="2">
         <v>-0.02</v>
@@ -3282,7 +3282,7 @@
         <v>0.66111111111111109</v>
       </c>
       <c r="E89" s="8">
-        <v>0.75555555555555554</v>
+        <v>0.75624999999999998</v>
       </c>
       <c r="F89" s="2">
         <v>0.02</v>

</xml_diff>